<commit_message>
Correction durée de retour sur invest. spécifique
</commit_message>
<xml_diff>
--- a/Dossier 4 - Choix de solution/Grille_d_evaluation_des_solutions_PLD_Spécifique.xlsx
+++ b/Dossier 4 - Choix de solution/Grille_d_evaluation_des_solutions_PLD_Spécifique.xlsx
@@ -151,9 +151,6 @@
     <t>32, Délai du retour sur investissement</t>
   </si>
   <si>
-    <t>6 mois</t>
-  </si>
-  <si>
     <t>II, Mise en œuvre</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>8 000/an + 75 000</t>
+  </si>
+  <si>
+    <t>4 mois</t>
   </si>
 </sst>
 </file>
@@ -440,13 +440,6 @@
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -544,6 +537,13 @@
     <xf numFmtId="4" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,41 +917,41 @@
   <dimension ref="A1:AMK51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.33203125" style="3"/>
-    <col min="2" max="2" width="16.77734375" style="3"/>
-    <col min="3" max="3" width="17.44140625" style="3"/>
-    <col min="4" max="4" width="17" style="3"/>
-    <col min="5" max="5" width="17" style="4"/>
-    <col min="6" max="6" width="45.6640625" style="4"/>
-    <col min="7" max="7" width="21.109375" style="3"/>
-    <col min="8" max="8" width="20.44140625" style="3"/>
-    <col min="9" max="1025" width="9.33203125" style="3"/>
+    <col min="1" max="1" width="72.33203125" style="1"/>
+    <col min="2" max="2" width="16.77734375" style="1"/>
+    <col min="3" max="3" width="17.44140625" style="1"/>
+    <col min="4" max="4" width="17" style="1"/>
+    <col min="5" max="5" width="17" style="2"/>
+    <col min="6" max="6" width="45.6640625" style="2"/>
+    <col min="7" max="7" width="21.109375" style="1"/>
+    <col min="8" max="8" width="20.44140625" style="1"/>
+    <col min="9" max="1025" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+    <row r="1" spans="1:1024" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:1024" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
@@ -1970,16 +1970,16 @@
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -2998,14 +2998,14 @@
       <c r="AMJ3"/>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
@@ -4024,16 +4024,16 @@
       <c r="AMJ4"/>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -6078,7 +6078,7 @@
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B7"/>
@@ -7106,7 +7106,7 @@
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8"/>
@@ -8134,7 +8134,7 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9"/>
@@ -9162,7 +9162,7 @@
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10"/>
@@ -10190,7 +10190,7 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B11"/>
@@ -11218,7 +11218,7 @@
       <c r="AMJ11"/>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
@@ -12243,491 +12243,491 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024" s="17" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:1024" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:1024" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23">
         <v>25000</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="s">
-        <v>79</v>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23" t="s">
+        <v>78</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23">
         <v>0</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23">
         <v>110000</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="24">
+      <c r="C24" s="25"/>
+      <c r="D24" s="22">
         <v>0</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="23">
         <v>0</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="1" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="39" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="1"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="1"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="25" t="s">
-        <v>45</v>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23" t="s">
+        <v>79</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="33"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="20" t="s">
+      <c r="F35" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="25" t="s">
+      <c r="F36" s="23" t="s">
         <v>52</v>
-      </c>
-      <c r="F36" s="25" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="25" t="s">
+      <c r="F37" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="25" t="s">
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="25"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="25" t="s">
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="25"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="25" t="s">
+      <c r="F40" s="23"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="25"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="25" t="s">
+      <c r="F41" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="F41" s="25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>66</v>
+      <c r="A42" s="32" t="s">
+        <v>65</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="25" t="s">
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="25" t="s">
-        <v>65</v>
+      <c r="F42" s="23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="31"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="33"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="20" t="s">
+      <c r="F45" s="19"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="25" t="s">
+      <c r="F46" s="23"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F46" s="25"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="25" t="s">
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F48" s="25"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="25" t="s">
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F49" s="25"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="23"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="F50" s="25"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="25" t="s">
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="25"/>
+      <c r="F51" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>